<commit_message>
JemTable & StringTable 수정
JemTable & StringTable 수정
</commit_message>
<xml_diff>
--- a/GameDesign/HMcsv설명/JemTable.xlsx
+++ b/GameDesign/HMcsv설명/JemTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82104\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82104\OneDrive\바탕 화면\github\Heros-Manager\GameDesign\HMcsv설명\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E2C765-5E37-446D-BCCF-E82D6C757F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F64CEB-8BE6-4466-A8B4-2BD1F44DB76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92ED02C7-F8F2-4A6C-93BA-6AAA5A997B06}"/>
+    <workbookView xWindow="7560" yWindow="924" windowWidth="13584" windowHeight="8964" xr2:uid="{92ED02C7-F8F2-4A6C-93BA-6AAA5A997B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>JemID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,6 +243,10 @@
   </si>
   <si>
     <t>Jem_MetalDetector_a1</t>
+  </si>
+  <si>
+    <t>StartLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -618,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047AD365-CA9B-4CF3-8630-19D803FED9C9}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -631,12 +635,13 @@
     <col min="3" max="3" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.69921875" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,16 +658,19 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -679,16 +687,19 @@
         <v>24</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.05</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -705,7 +716,7 @@
         <v>25</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -713,8 +724,11 @@
       <c r="H3">
         <v>3</v>
       </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -731,16 +745,19 @@
         <v>26</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -757,12 +774,15 @@
         <v>27</v>
       </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.03</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>